<commit_message>
Fix one dud transcribed position
</commit_message>
<xml_diff>
--- a/voyages/endurance_1914-6/as_digitised/AURORA 1914-1915.xlsx
+++ b/voyages/endurance_1914-6/as_digitised/AURORA 1914-1915.xlsx
@@ -1190,8 +1190,8 @@
   <dimension ref="A2:O4530"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="5" topLeftCell="A378" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="B3" sqref="B3"/>
+      <pane ySplit="5" topLeftCell="A423" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H438" sqref="H438"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -8817,7 +8817,7 @@
         <v>14</v>
       </c>
       <c r="H438">
-        <v>149.31</v>
+        <v>169.31</v>
       </c>
       <c r="I438">
         <v>169.45</v>

</xml_diff>